<commit_message>
Fixed y polarization and added values
</commit_message>
<xml_diff>
--- a/tracking_optimization.xlsx
+++ b/tracking_optimization.xlsx
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J2" sqref="J2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -422,13 +422,13 @@
         <v>-1.0920000000000001</v>
       </c>
       <c r="B2">
-        <v>0.35625000000000001</v>
+        <v>-0.35625000000000001</v>
       </c>
       <c r="C2">
         <v>1.2495000000000001</v>
       </c>
       <c r="D2">
-        <v>-0.74099999999999999</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="F2">
         <v>12500</v>
@@ -438,15 +438,6 @@
       </c>
       <c r="H2">
         <v>7320</v>
-      </c>
-      <c r="J2">
-        <v>33652</v>
-      </c>
-      <c r="K2">
-        <v>7195</v>
-      </c>
-      <c r="L2">
-        <v>5950</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -454,13 +445,13 @@
         <v>-1.9319999999999999</v>
       </c>
       <c r="B3">
-        <v>1.0069999999999999</v>
+        <v>-1.0069999999999999</v>
       </c>
       <c r="C3">
         <v>0.87849999999999995</v>
       </c>
       <c r="D3">
-        <v>-1.0545</v>
+        <v>1.0545</v>
       </c>
       <c r="F3">
         <v>12500</v>
@@ -470,15 +461,6 @@
       </c>
       <c r="H3">
         <v>4880</v>
-      </c>
-      <c r="J3">
-        <v>34799</v>
-      </c>
-      <c r="K3">
-        <v>11943</v>
-      </c>
-      <c r="L3">
-        <v>12005</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -486,13 +468,13 @@
         <v>-1.0009999999999999</v>
       </c>
       <c r="B4">
-        <v>6.1749999999999999E-2</v>
+        <v>-6.1749999999999999E-2</v>
       </c>
       <c r="C4">
         <v>0.15049999999999999</v>
       </c>
       <c r="D4">
-        <v>-0.30399999999999999</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="F4">
         <v>15000</v>
@@ -502,15 +484,6 @@
       </c>
       <c r="H4">
         <v>2440</v>
-      </c>
-      <c r="J4">
-        <v>28915</v>
-      </c>
-      <c r="K4">
-        <v>4828</v>
-      </c>
-      <c r="L4">
-        <v>6569</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -518,13 +491,13 @@
         <v>0.1925</v>
       </c>
       <c r="B5">
-        <v>-7.1249999999999994E-2</v>
+        <v>7.1249999999999994E-2</v>
       </c>
       <c r="C5">
         <v>0.92749999999999999</v>
       </c>
       <c r="D5">
-        <v>-7.5999999999999998E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="F5">
         <v>15000</v>
@@ -534,15 +507,6 @@
       </c>
       <c r="H5">
         <v>7320</v>
-      </c>
-      <c r="J5">
-        <v>25058</v>
-      </c>
-      <c r="K5">
-        <v>3825</v>
-      </c>
-      <c r="L5">
-        <v>-800</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -550,13 +514,13 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="B6">
-        <v>-0.69350000000000001</v>
+        <v>0.69350000000000001</v>
       </c>
       <c r="C6">
         <v>0.217</v>
       </c>
       <c r="D6">
-        <v>1.0069999999999999</v>
+        <v>-1.0069999999999999</v>
       </c>
       <c r="F6">
         <v>20000</v>
@@ -566,15 +530,6 @@
       </c>
       <c r="H6">
         <v>4880</v>
-      </c>
-      <c r="J6">
-        <v>21855</v>
-      </c>
-      <c r="K6">
-        <v>48</v>
-      </c>
-      <c r="L6">
-        <v>1223</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -582,13 +537,13 @@
         <v>-0.71314999999999995</v>
       </c>
       <c r="B7">
-        <v>-1.4724999999999999</v>
+        <v>1.4724999999999999</v>
       </c>
       <c r="C7">
         <v>0.224</v>
       </c>
       <c r="D7">
-        <v>0.96250000000000002</v>
+        <v>-0.96250000000000002</v>
       </c>
       <c r="F7">
         <v>15000</v>
@@ -598,15 +553,6 @@
       </c>
       <c r="H7">
         <v>2440</v>
-      </c>
-      <c r="J7">
-        <v>24272</v>
-      </c>
-      <c r="K7">
-        <v>-4599</v>
-      </c>
-      <c r="L7">
-        <v>6343</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -614,13 +560,13 @@
         <v>0.308</v>
       </c>
       <c r="B8">
-        <v>-1.2017500000000001</v>
+        <v>1.2017500000000001</v>
       </c>
       <c r="C8">
         <v>0.91700000000000004</v>
       </c>
       <c r="D8">
-        <v>0.78374999999999995</v>
+        <v>-0.78374999999999995</v>
       </c>
       <c r="F8">
         <v>15000</v>
@@ -631,14 +577,51 @@
       <c r="H8">
         <v>7320</v>
       </c>
-      <c r="J8">
-        <v>23417</v>
-      </c>
-      <c r="K8">
-        <v>-3748</v>
-      </c>
-      <c r="L8">
-        <v>-670</v>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>-0.371</v>
+      </c>
+      <c r="B9">
+        <v>0.25174999999999997</v>
+      </c>
+      <c r="C9">
+        <v>0.52849999999999997</v>
+      </c>
+      <c r="D9">
+        <v>-1.4250000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>15000</v>
+      </c>
+      <c r="G9">
+        <v>5000</v>
+      </c>
+      <c r="H9">
+        <v>4880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>-1.3049999999999999</v>
+      </c>
+      <c r="B10">
+        <v>1.3347500000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.87150000000000005</v>
+      </c>
+      <c r="D10">
+        <v>-0.20424999999999999</v>
+      </c>
+      <c r="F10">
+        <v>12500</v>
+      </c>
+      <c r="G10">
+        <v>7500</v>
+      </c>
+      <c r="H10">
+        <v>4880</v>
       </c>
     </row>
   </sheetData>

</xml_diff>